<commit_message>
Paper sent to Athena for review
</commit_message>
<xml_diff>
--- a/data/complete/consolidated/journal_data_policies_both.xlsx
+++ b/data/complete/consolidated/journal_data_policies_both.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/lm16564_bristol_ac_uk/Documents/Documents/rrr/data-availability-impact/data/complete/consolidated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="222" documentId="8_{521659CC-55AA-4A3B-9F81-3393CC832DE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A75B0B20-6FDC-4F42-B4F1-5670E8CBCD2E}"/>
+  <xr:revisionPtr revIDLastSave="227" documentId="8_{521659CC-55AA-4A3B-9F81-3393CC832DE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{859597AB-7F02-4FE1-9042-000178FDEBA7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{207352FD-B52B-4F8B-A157-E55A47A6431A}"/>
   </bookViews>
@@ -1147,9 +1147,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1466,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F96BA9-A474-44F2-95FC-F5C628E1CBD7}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,11 +1815,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C17" s="1">
@@ -3397,21 +3400,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AB879562A5253941BC4792E4BFFA7253" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1136095aeba14c76d3b5daf33cacb3d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="50c6f0d6-8741-4da4-b08f-402b0ce19755" xmlns:ns4="29791920-2275-484b-95df-8920050dfdd8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0368936cfa1d9e469dc08934c908f5f6" ns3:_="" ns4:_="">
     <xsd:import namespace="50c6f0d6-8741-4da4-b08f-402b0ce19755"/>
@@ -3634,24 +3622,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E353106-99AB-4DFE-8101-F7DE1BBD5F28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DC53147-4E97-4C87-8013-A818B8A65A6E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D17779D1-F9CF-4C20-A20D-440E62B507AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3668,4 +3654,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DC53147-4E97-4C87-8013-A818B8A65A6E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E353106-99AB-4DFE-8101-F7DE1BBD5F28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>